<commit_message>
Modified placeData method such that all equations are calculated
</commit_message>
<xml_diff>
--- a/toFill.xlsx
+++ b/toFill.xlsx
@@ -1,34 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FNORD\Desktop\Projects\Finance\dividendTracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E73AB47-239B-4817-8EFD-95C0B578C4B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dividend calc" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="dividend calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+  <si>
+    <t>Stock ID</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>Annual Yield</t>
+  </si>
+  <si>
+    <t>$stock/$div</t>
+  </si>
+  <si>
+    <t>$stock/$annual</t>
+  </si>
+  <si>
+    <t>Annual yield for $1k</t>
+  </si>
+  <si>
+    <t>Updated:</t>
+  </si>
+  <si>
+    <t>2019-07-20 07:45:44.998184</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>2.72</t>
+  </si>
+  <si>
+    <t>uuuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A </t>
+  </si>
+  <si>
+    <t>roku</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>2.04</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,15 +112,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,94 +417,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Stock ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Yield</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Recurrence</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Yield</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Annual Yield</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>$stock/$div</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>$stock/$annual</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Annual yield for $1k</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Updated:</t>
-        </is>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>107.6600036621094</v>
+      </c>
       <c r="C2">
         <f>F2/B2</f>
-        <v/>
+        <v>2.5264721414432718E-2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
       </c>
       <c r="E2">
         <f>F2/D2</f>
-        <v/>
+        <v>0.68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
       <c r="G2">
         <f>B2/E2</f>
-        <v/>
+        <v>158.32353479721971</v>
       </c>
       <c r="H2">
         <f>B2/F2</f>
-        <v/>
+        <v>39.580883699304927</v>
       </c>
       <c r="I2">
-        <f>FLOOR.MATH(1000/B2)*F2</f>
-        <v/>
+        <f>_xlfn.FLOOR.MATH(1000/B2)*F2</f>
+        <v>24.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>1.970000028610229</v>
+      </c>
+      <c r="C3" t="e">
+        <f>F3/B3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="e">
+        <f>F3/D3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="e">
+        <f>B3/E3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" t="e">
+        <f>B3/F3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" t="e">
+        <f>_xlfn.FLOOR.MATH(1000/B3)*F3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>106.84999847412109</v>
+      </c>
+      <c r="C4" t="e">
+        <f>F4/B4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="e">
+        <f>F4/D4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="e">
+        <f>B4/E4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4" t="e">
+        <f>B4/F4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" t="e">
+        <f>_xlfn.FLOOR.MATH(1000/B4)*F4</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>32.790000915527337</v>
+      </c>
+      <c r="C5">
+        <f>F5/B5</f>
+        <v>6.2214087924406886E-2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>F5/D5</f>
+        <v>0.51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <f>B5/E5</f>
+        <v>64.294119442210459</v>
+      </c>
+      <c r="H5">
+        <f>B5/F5</f>
+        <v>16.073529860552615</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.FLOOR.MATH(1000/B5)*F5</f>
+        <v>61.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified new and placeData methods for streamlined sheet layout
</commit_message>
<xml_diff>
--- a/toFill.xlsx
+++ b/toFill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FNORD\Desktop\Projects\Finance\dividendTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E73AB47-239B-4817-8EFD-95C0B578C4B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33301A-9A26-4DA2-A5FA-F986E3D8FE18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Stock ID</t>
   </si>
@@ -39,46 +39,19 @@
     <t>Yield</t>
   </si>
   <si>
-    <t>Recurrence</t>
-  </si>
-  <si>
     <t>Annual Yield</t>
   </si>
   <si>
-    <t>$stock/$div</t>
-  </si>
-  <si>
-    <t>$stock/$annual</t>
-  </si>
-  <si>
-    <t>Annual yield for $1k</t>
+    <t>2019-07-30 08:50:26.785769</t>
   </si>
   <si>
     <t>Updated:</t>
   </si>
   <si>
-    <t>2019-07-20 07:45:44.998184</t>
-  </si>
-  <si>
-    <t>has</t>
-  </si>
-  <si>
-    <t>2.72</t>
-  </si>
-  <si>
-    <t>uuuu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A </t>
-  </si>
-  <si>
-    <t>roku</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>2.04</t>
+    <t>$price/annual yield</t>
+  </si>
+  <si>
+    <t>Annual Yield for $1k</t>
   </si>
 </sst>
 </file>
@@ -418,15 +391,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.9453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,161 +423,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>107.6600036621094</v>
-      </c>
-      <c r="C2">
-        <f>F2/B2</f>
-        <v>2.5264721414432718E-2</v>
-      </c>
-      <c r="D2">
         <v>4</v>
-      </c>
-      <c r="E2">
-        <f>F2/D2</f>
-        <v>0.68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <f>B2/E2</f>
-        <v>158.32353479721971</v>
-      </c>
-      <c r="H2">
-        <f>B2/F2</f>
-        <v>39.580883699304927</v>
-      </c>
-      <c r="I2">
-        <f>_xlfn.FLOOR.MATH(1000/B2)*F2</f>
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>1.970000028610229</v>
-      </c>
-      <c r="C3" t="e">
-        <f>F3/B3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3" t="e">
-        <f>F3/D3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="e">
-        <f>B3/E3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" t="e">
-        <f>B3/F3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I3" t="e">
-        <f>_xlfn.FLOOR.MATH(1000/B3)*F3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>106.84999847412109</v>
-      </c>
-      <c r="C4" t="e">
-        <f>F4/B4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="e">
-        <f>F4/D4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="e">
-        <f>B4/E4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H4" t="e">
-        <f>B4/F4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I4" t="e">
-        <f>_xlfn.FLOOR.MATH(1000/B4)*F4</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>32.790000915527337</v>
-      </c>
-      <c r="C5">
-        <f>F5/B5</f>
-        <v>6.2214087924406886E-2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f>F5/D5</f>
-        <v>0.51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <f>B5/E5</f>
-        <v>64.294119442210459</v>
-      </c>
-      <c r="H5">
-        <f>B5/F5</f>
-        <v>16.073529860552615</v>
-      </c>
-      <c r="I5">
-        <f>_xlfn.FLOOR.MATH(1000/B5)*F5</f>
-        <v>61.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>